<commit_message>
working through siskiyou fertilizer
</commit_message>
<xml_diff>
--- a/R/data_refs/refbyhand_fert-types.xlsx
+++ b/R/data_refs/refbyhand_fert-types.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gina\Documents\_git-it\alfalfa\R\data_refs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EEA471F3-E26B-4F5F-83E1-9B0F219B2D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF69D3E-304C-4D13-8040-C703A8236C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31965" yWindow="1350" windowWidth="21600" windowHeight="11325" xr2:uid="{F9C204EB-B1FD-42C0-A116-E7E2A0D8614D}"/>
+    <workbookView xWindow="3945" yWindow="2385" windowWidth="21600" windowHeight="11265" xr2:uid="{F9C204EB-B1FD-42C0-A116-E7E2A0D8614D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>fert_type</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>this is the 'master' label</t>
+  </si>
+  <si>
+    <t>sulfur</t>
+  </si>
+  <si>
+    <t>potassium</t>
+  </si>
+  <si>
+    <t>sodium molybdate</t>
   </si>
 </sst>
 </file>
@@ -405,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB40291F-D8CB-46D7-BB80-2F26A0D02830}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,6 +452,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>